<commit_message>
Farmer choose crop based on expected profit
</commit_message>
<xml_diff>
--- a/crops_info.xlsx
+++ b/crops_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\irrigation_abm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC79675F-26E8-4AD1-B13E-BD0DFC51D7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B92ED92-DB9C-46FD-B313-19BD182598CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="4305" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Maize</t>
   </si>
@@ -43,13 +43,16 @@
     <t>Passion Fruit</t>
   </si>
   <si>
-    <t>Tobacco</t>
-  </si>
-  <si>
-    <t>efficiency</t>
-  </si>
-  <si>
-    <t>yield_per_ton</t>
+    <t>Cassava</t>
+  </si>
+  <si>
+    <t>Revenue (R$/ton)</t>
+  </si>
+  <si>
+    <t>Cost (R$/ton)</t>
+  </si>
+  <si>
+    <t>Yield (ton/ha)</t>
   </si>
 </sst>
 </file>
@@ -367,15 +370,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -392,30 +395,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>1924</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="C2">
-        <v>14428</v>
+        <v>14.428000000000001</v>
       </c>
       <c r="D2">
-        <v>1228</v>
+        <v>11.391999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>664</v>
+      </c>
+      <c r="C3">
+        <v>1845</v>
+      </c>
+      <c r="D3">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>664.21462570315884</v>
-      </c>
-      <c r="C3">
-        <v>1845.2484742807324</v>
-      </c>
-      <c r="D3">
-        <v>11632.785067455185</v>
+      <c r="B4">
+        <v>448</v>
+      </c>
+      <c r="C4">
+        <v>1351</v>
+      </c>
+      <c r="D4">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>